<commit_message>
fixed fuel tax rebatements for germany and france, storage data and german policy
</commit_message>
<xml_diff>
--- a/data/_master-data/fuel data - 2023.xlsx
+++ b/data/_master-data/fuel data - 2023.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\GitHub\PhD\J4 - model\data\_master-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C435D527-7CC1-406A-9E1D-83E7BEA78E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E226C7-4EDF-4C84-91EB-0CE490C0FFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6E05FBF9-7A0C-4B38-8AD0-297E8124D7D0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6E05FBF9-7A0C-4B38-8AD0-297E8124D7D0}"/>
   </bookViews>
   <sheets>
     <sheet name="DE" sheetId="5" r:id="rId1"/>
     <sheet name="DK" sheetId="6" r:id="rId2"/>
     <sheet name="FR" sheetId="7" r:id="rId3"/>
-    <sheet name="fuel data - DK (original)" sheetId="3" r:id="rId4"/>
+    <sheet name="FR_gentax" sheetId="8" r:id="rId4"/>
+    <sheet name="fuel data - DK (original)" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>biogas</t>
   </si>
@@ -261,6 +262,33 @@
   </si>
   <si>
     <t>Excemtion for CHP is implemented in other input file</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>HCV7</t>
+  </si>
+  <si>
+    <t>HCV8</t>
+  </si>
+  <si>
+    <t>Tax factor</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>beta_b</t>
+  </si>
+  <si>
+    <t>reduction rate</t>
+  </si>
+  <si>
+    <t>normal tax</t>
+  </si>
+  <si>
+    <t>tax reduction</t>
   </si>
 </sst>
 </file>
@@ -375,14 +403,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,278 +729,278 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="12.5703125" style="22"/>
-    <col min="7" max="7" width="132.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="22"/>
+    <col min="1" max="6" width="12.5703125" style="20"/>
+    <col min="7" max="7" width="132.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.5703125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <v>67.730999999999995</v>
       </c>
-      <c r="C2" s="22">
-        <v>0</v>
-      </c>
-      <c r="D2" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E2" s="22">
-        <v>0</v>
-      </c>
-      <c r="F2" s="22">
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E2" s="20">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <v>33.406999999999996</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <v>338.76</v>
       </c>
-      <c r="D3" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E3" s="22">
+      <c r="D3" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E3" s="20">
         <v>1.1879999999999999</v>
       </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E4" s="22">
+      <c r="D4" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E4" s="20">
         <v>20.5</v>
       </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22">
-        <v>0</v>
-      </c>
-      <c r="D5" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E5" s="22">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
+      <c r="B5" s="20">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0</v>
+      </c>
+      <c r="D5" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>49.966000000000001</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="20">
         <v>285.48</v>
       </c>
-      <c r="D6" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="D6" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E6" s="20">
         <v>2.2726999999999999</v>
       </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>91.096999999999994</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <v>266.76</v>
       </c>
-      <c r="D7" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E7" s="22">
+      <c r="D7" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E7" s="20">
         <v>4.7085999999999997</v>
       </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>-19.122</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="20">
         <v>153</v>
       </c>
-      <c r="D8" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E8" s="22">
-        <v>0</v>
-      </c>
-      <c r="F8" s="22">
-        <v>0</v>
-      </c>
-      <c r="G8" s="22" t="s">
+      <c r="D8" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>146.66200000000001</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <v>203.4</v>
       </c>
-      <c r="D9" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E9" s="22">
+      <c r="D9" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E9" s="20">
         <v>5.5</v>
       </c>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="20">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>47.697000000000003</v>
       </c>
-      <c r="C10" s="22">
-        <v>0</v>
-      </c>
-      <c r="D10" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22">
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>76.662000000000006</v>
       </c>
-      <c r="C11" s="22">
-        <v>0</v>
-      </c>
-      <c r="D11" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0</v>
-      </c>
-      <c r="F11" s="22">
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>12.069000000000001</v>
       </c>
-      <c r="C12" s="22">
-        <v>0</v>
-      </c>
-      <c r="D12" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+      <c r="D12" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -985,272 +1013,272 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBFAED8-3004-4207-A0C6-701BFA650063}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="12.5703125" style="22"/>
-    <col min="7" max="7" width="99.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="22"/>
+    <col min="1" max="6" width="12.5703125" style="20"/>
+    <col min="7" max="7" width="99.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.5703125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <v>67.730999999999995</v>
       </c>
-      <c r="C2" s="22">
-        <v>0</v>
-      </c>
-      <c r="D2" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E2" s="22">
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E2" s="20">
         <v>2.0617000000000001</v>
       </c>
-      <c r="F2" s="22">
-        <v>0</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="20">
+        <v>0</v>
+      </c>
+      <c r="G2" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <v>33.406999999999996</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <v>338.76</v>
       </c>
-      <c r="D3" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E3" s="22">
+      <c r="D3" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E3" s="20">
         <v>30.893000000000001</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E4" s="22">
+      <c r="D4" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E4" s="20">
         <v>92.472999999999999</v>
       </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22">
-        <v>0</v>
-      </c>
-      <c r="D5" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E5" s="22">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22" t="s">
+      <c r="B5" s="20">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0</v>
+      </c>
+      <c r="D5" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>49.966000000000001</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="20">
         <v>285.48</v>
       </c>
-      <c r="D6" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="D6" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E6" s="20">
         <v>29.501999999999999</v>
       </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>91.096999999999994</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <v>266.76</v>
       </c>
-      <c r="D7" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E7" s="22">
+      <c r="D7" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E7" s="20">
         <v>37.378</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>-19.122</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="20">
         <v>153</v>
       </c>
-      <c r="D8" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E8" s="22">
-        <v>0</v>
-      </c>
-      <c r="F8" s="22">
+      <c r="D8" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>146.66200000000001</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <v>203.4</v>
       </c>
-      <c r="D9" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E9" s="22">
+      <c r="D9" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E9" s="20">
         <v>35.889000000000003</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>47.697000000000003</v>
       </c>
-      <c r="C10" s="22">
-        <v>0</v>
-      </c>
-      <c r="D10" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22">
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>76.662000000000006</v>
       </c>
-      <c r="C11" s="22">
-        <v>0</v>
-      </c>
-      <c r="D11" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0</v>
-      </c>
-      <c r="F11" s="22">
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>12.069000000000001</v>
       </c>
-      <c r="C12" s="22">
-        <v>0</v>
-      </c>
-      <c r="D12" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+      <c r="D12" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1264,277 +1292,277 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="12.5703125" style="22"/>
-    <col min="7" max="7" width="67.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="22"/>
+    <col min="1" max="6" width="12.5703125" style="20"/>
+    <col min="7" max="7" width="67.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.5703125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <v>67.730999999999995</v>
       </c>
-      <c r="C2" s="22">
-        <v>0</v>
-      </c>
-      <c r="D2" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E2" s="22">
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E2" s="20">
         <v>1.196</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="20">
         <v>33.406999999999996</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="20">
         <v>338.76</v>
       </c>
-      <c r="D3" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E3" s="22">
+      <c r="D3" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E3" s="20">
         <v>14.62</v>
       </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="22" t="s">
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E4" s="22">
+      <c r="D4" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E4" s="20">
         <v>21</v>
       </c>
-      <c r="F4" s="22">
-        <v>0</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="22">
-        <v>0</v>
-      </c>
-      <c r="C5" s="22">
-        <v>0</v>
-      </c>
-      <c r="D5" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E5" s="22">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
+      <c r="B5" s="20">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0</v>
+      </c>
+      <c r="D5" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="20">
         <v>49.966000000000001</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="20">
         <v>285.48</v>
       </c>
-      <c r="D6" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="D6" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E6" s="20">
         <v>12.555</v>
       </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>91.096999999999994</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <v>266.76</v>
       </c>
-      <c r="D7" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E7" s="22">
+      <c r="D7" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E7" s="20">
         <v>5.1890000000000001</v>
       </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22" t="s">
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="20">
         <v>-19.122</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="20">
         <v>153</v>
       </c>
-      <c r="D8" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E8" s="22">
-        <v>0</v>
-      </c>
-      <c r="F8" s="22">
+      <c r="D8" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="20">
         <v>146.66200000000001</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="20">
         <v>203.4</v>
       </c>
-      <c r="D9" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E9" s="22">
+      <c r="D9" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E9" s="20">
         <v>8.3699999999999992</v>
       </c>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
-      <c r="G9" s="22" t="s">
+      <c r="F9" s="20">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="20">
         <v>47.697000000000003</v>
       </c>
-      <c r="C10" s="22">
-        <v>0</v>
-      </c>
-      <c r="D10" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22">
+      <c r="C10" s="20">
+        <v>0</v>
+      </c>
+      <c r="D10" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="20">
         <v>76.662000000000006</v>
       </c>
-      <c r="C11" s="22">
-        <v>0</v>
-      </c>
-      <c r="D11" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E11" s="22">
-        <v>0</v>
-      </c>
-      <c r="F11" s="22">
+      <c r="C11" s="20">
+        <v>0</v>
+      </c>
+      <c r="D11" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="20">
         <v>12.069000000000001</v>
       </c>
-      <c r="C12" s="22">
-        <v>0</v>
-      </c>
-      <c r="D12" s="22">
-        <v>8.5300000000000001E-2</v>
-      </c>
-      <c r="E12" s="22">
-        <v>0</v>
-      </c>
-      <c r="F12" s="22">
+      <c r="C12" s="20">
+        <v>0</v>
+      </c>
+      <c r="D12" s="20">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1544,6 +1572,99 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A79BF222-0945-4F13-86DA-E9843496BD6E}">
+  <dimension ref="B2:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>1.3</v>
+      </c>
+      <c r="D5">
+        <v>0.89</v>
+      </c>
+      <c r="E5">
+        <v>0.41</v>
+      </c>
+      <c r="F5">
+        <f>C5*D5*(E5/(E5+1))</f>
+        <v>0.33643262411347513</v>
+      </c>
+      <c r="G5" s="20">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="H5">
+        <f>-ROUND(F5*G5,2)</f>
+        <v>-2.82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>1.3</v>
+      </c>
+      <c r="D6">
+        <v>0.89</v>
+      </c>
+      <c r="E6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F6">
+        <f>C6*D6*(E6/(E6+1))</f>
+        <v>0.26010077519379843</v>
+      </c>
+      <c r="G6">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="H6">
+        <f>-ROUND(F6*G6,2)</f>
+        <v>-2.1800000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931181A0-02B4-4BE8-AAB8-3DB7EDEE65B2}">
   <dimension ref="A1:P17"/>
   <sheetViews>
@@ -1598,27 +1719,27 @@
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20" t="s">
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="20"/>
+      <c r="L5" s="22"/>
       <c r="M5" s="14" t="s">
         <v>27</v>
       </c>

</xml_diff>